<commit_message>
update xls and xml files
after fixing the "keys" for options in both files, replacing them
</commit_message>
<xml_diff>
--- a/survey_resources/washingtoncommons/washingtoncommons-onboarding-survey.xlsx
+++ b/survey_resources/washingtoncommons/washingtoncommons-onboarding-survey.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awheelis/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77599B24-5385-A145-98E9-A0C54946A276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-2180" yWindow="-18940" windowWidth="31200" windowHeight="16600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="choices" sheetId="2" r:id="rId2"/>
     <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="401">
   <si>
     <t>type</t>
   </si>
@@ -564,10 +570,7 @@
     <t>go8ys98</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve">No </t>
+    <t>No </t>
   </si>
   <si>
     <t>wz77v03</t>
@@ -726,15 +729,9 @@
     <t>nj2og72</t>
   </si>
   <si>
-    <t>option_1</t>
-  </si>
-  <si>
     <t>Less than $20,000</t>
   </si>
   <si>
-    <t>option_2</t>
-  </si>
-  <si>
     <t>$20,000 to $34,999</t>
   </si>
   <si>
@@ -846,9 +843,6 @@
     <t>Widowed</t>
   </si>
   <si>
-    <t>option_5</t>
-  </si>
-  <si>
     <t>kg1ne48</t>
   </si>
   <si>
@@ -978,9 +972,6 @@
     <t>Three</t>
   </si>
   <si>
-    <t>option_4</t>
-  </si>
-  <si>
     <t xml:space="preserve">Four and more </t>
   </si>
   <si>
@@ -1002,7 +993,7 @@
     <t>neutral</t>
   </si>
   <si>
-    <t xml:space="preserve">Neutral </t>
+    <t>Neutral </t>
   </si>
   <si>
     <t>agree</t>
@@ -1011,7 +1002,7 @@
     <t>strongly_agree</t>
   </si>
   <si>
-    <t xml:space="preserve">strongly agree </t>
+    <t>strongly agree </t>
   </si>
   <si>
     <t>dg8at95</t>
@@ -1029,9 +1020,6 @@
     <t>Sometimes I feel unsafe when traveling.</t>
   </si>
   <si>
-    <t>option_3</t>
-  </si>
-  <si>
     <t>I often feel unsafe when traveling.</t>
   </si>
   <si>
@@ -1174,13 +1162,76 @@
   </si>
   <si>
     <t>lg13m77</t>
+  </si>
+  <si>
+    <t>_20_000_to_34_999</t>
+  </si>
+  <si>
+    <t>_less_than_20_000</t>
+  </si>
+  <si>
+    <t>four_or_more</t>
+  </si>
+  <si>
+    <t>i_often_feel_unsafe_when_traveling</t>
+  </si>
+  <si>
+    <t>usually_takes_too_long</t>
+  </si>
+  <si>
+    <t>sometimes_takes_too_long</t>
+  </si>
+  <si>
+    <t>often_go_quickly</t>
+  </si>
+  <si>
+    <t>always_hard</t>
+  </si>
+  <si>
+    <t>sometimes_hard</t>
+  </si>
+  <si>
+    <t>usually_easy</t>
+  </si>
+  <si>
+    <t>usually_pleasant</t>
+  </si>
+  <si>
+    <t>sometimes_pleasant</t>
+  </si>
+  <si>
+    <t>often_unpleasant</t>
+  </si>
+  <si>
+    <t>usually_afford</t>
+  </si>
+  <si>
+    <t>sometimes_afford</t>
+  </si>
+  <si>
+    <t>never_afford</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>smaller</t>
+  </si>
+  <si>
+    <t>larger</t>
+  </si>
+  <si>
+    <t>under_6</t>
+  </si>
+  <si>
+    <t>strongly_disagree</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1217,13 +1268,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1261,7 +1320,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1295,6 +1354,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1329,9 +1389,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1504,14 +1565,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="5" width="40.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1528,7 +1594,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1536,7 +1602,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1544,7 +1610,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1558,7 +1624,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1569,7 +1635,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1583,7 +1649,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1600,7 +1666,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1617,7 +1683,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1634,7 +1700,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1651,7 +1717,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1668,12 +1734,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1684,7 +1750,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -1701,7 +1767,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1718,7 +1784,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -1735,7 +1801,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -1752,12 +1818,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -1768,7 +1834,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -1785,7 +1851,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -1802,7 +1868,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -1819,7 +1885,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -1836,12 +1902,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -1852,7 +1918,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1869,7 +1935,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -1886,7 +1952,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -1903,7 +1969,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>48</v>
       </c>
@@ -1920,12 +1986,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>11</v>
       </c>
@@ -1936,7 +2002,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -1953,7 +2019,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>42</v>
       </c>
@@ -1970,7 +2036,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -1987,7 +2053,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>48</v>
       </c>
@@ -2004,12 +2070,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -2020,7 +2086,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>29</v>
       </c>
@@ -2037,7 +2103,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -2054,7 +2120,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -2071,7 +2137,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>48</v>
       </c>
@@ -2088,12 +2154,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>79</v>
       </c>
@@ -2107,7 +2173,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>82</v>
       </c>
@@ -2121,7 +2187,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>85</v>
       </c>
@@ -2135,7 +2201,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>88</v>
       </c>
@@ -2149,7 +2215,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>91</v>
       </c>
@@ -2163,7 +2229,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>94</v>
       </c>
@@ -2177,7 +2243,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>97</v>
       </c>
@@ -2191,7 +2257,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>100</v>
       </c>
@@ -2205,7 +2271,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>103</v>
       </c>
@@ -2219,7 +2285,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>11</v>
       </c>
@@ -2230,7 +2296,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>107</v>
       </c>
@@ -2244,7 +2310,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>107</v>
       </c>
@@ -2261,7 +2327,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>107</v>
       </c>
@@ -2278,7 +2344,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>107</v>
       </c>
@@ -2295,7 +2361,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>107</v>
       </c>
@@ -2312,7 +2378,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>107</v>
       </c>
@@ -2329,7 +2395,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>107</v>
       </c>
@@ -2346,7 +2412,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>107</v>
       </c>
@@ -2363,12 +2429,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>124</v>
       </c>
@@ -2382,7 +2448,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>127</v>
       </c>
@@ -2396,7 +2462,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>130</v>
       </c>
@@ -2410,7 +2476,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>11</v>
       </c>
@@ -2421,7 +2487,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>134</v>
       </c>
@@ -2435,7 +2501,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>134</v>
       </c>
@@ -2452,7 +2518,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>134</v>
       </c>
@@ -2469,7 +2535,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>134</v>
       </c>
@@ -2486,7 +2552,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>134</v>
       </c>
@@ -2503,7 +2569,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>134</v>
       </c>
@@ -2520,7 +2586,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>134</v>
       </c>
@@ -2537,12 +2603,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>29</v>
       </c>
@@ -2556,7 +2622,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>151</v>
       </c>
@@ -2570,7 +2636,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>154</v>
       </c>
@@ -2584,7 +2650,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>157</v>
       </c>
@@ -2598,7 +2664,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>159</v>
       </c>
@@ -2612,7 +2678,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>161</v>
       </c>
@@ -2626,7 +2692,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>163</v>
       </c>
@@ -2640,7 +2706,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>166</v>
       </c>
@@ -2654,7 +2720,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>169</v>
       </c>
@@ -2668,7 +2734,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>172</v>
       </c>
@@ -2688,14 +2754,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C117"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="3" width="40.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>175</v>
       </c>
@@ -2706,7 +2777,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>176</v>
       </c>
@@ -2717,7 +2788,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>176</v>
       </c>
@@ -2728,18 +2799,18 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>181</v>
       </c>
       <c r="B4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C4" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>181</v>
       </c>
@@ -2747,672 +2818,672 @@
         <v>179</v>
       </c>
       <c r="C5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>184</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>185</v>
       </c>
-      <c r="C6" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>183</v>
+      </c>
+      <c r="B7" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>184</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>187</v>
       </c>
-      <c r="C7" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B8" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>184</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>189</v>
       </c>
-      <c r="C8" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>183</v>
+      </c>
+      <c r="B9" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>184</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>191</v>
       </c>
-      <c r="C9" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
         <v>193</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>194</v>
       </c>
-      <c r="C10" t="s">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>192</v>
+      </c>
+      <c r="B11" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>193</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>196</v>
       </c>
-      <c r="C11" t="s">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>192</v>
+      </c>
+      <c r="B12" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>193</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>198</v>
       </c>
-      <c r="C12" t="s">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>192</v>
+      </c>
+      <c r="B13" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>193</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>200</v>
       </c>
-      <c r="C13" t="s">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
         <v>202</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>203</v>
       </c>
-      <c r="C14" t="s">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>201</v>
+      </c>
+      <c r="B15" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>202</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>205</v>
       </c>
-      <c r="C15" t="s">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>201</v>
+      </c>
+      <c r="B16" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>202</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>207</v>
       </c>
-      <c r="C16" t="s">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>201</v>
+      </c>
+      <c r="B17" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>202</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>209</v>
       </c>
-      <c r="C17" t="s">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
         <v>211</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>212</v>
       </c>
-      <c r="C18" t="s">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>210</v>
+      </c>
+      <c r="B19" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>211</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>214</v>
       </c>
-      <c r="C19" t="s">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>210</v>
+      </c>
+      <c r="B20" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>211</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>216</v>
       </c>
-      <c r="C20" t="s">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>210</v>
+      </c>
+      <c r="B21" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>211</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>218</v>
       </c>
-      <c r="C21" t="s">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>210</v>
+      </c>
+      <c r="B22" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>211</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>220</v>
       </c>
-      <c r="C22" t="s">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>210</v>
+      </c>
+      <c r="B23" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>211</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>222</v>
       </c>
-      <c r="C23" t="s">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>210</v>
+      </c>
+      <c r="B24" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>211</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>224</v>
       </c>
-      <c r="C24" t="s">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
+      <c r="B25" t="s">
         <v>226</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>227</v>
       </c>
-      <c r="C25" t="s">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>225</v>
+      </c>
+      <c r="B26" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
-        <v>226</v>
-      </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>229</v>
       </c>
-      <c r="C26" t="s">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>225</v>
+      </c>
+      <c r="B27" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
-        <v>226</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>231</v>
       </c>
-      <c r="C27" t="s">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>225</v>
+      </c>
+      <c r="B28" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
-        <v>226</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>233</v>
       </c>
-      <c r="C28" t="s">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
+      <c r="B29" t="s">
+        <v>381</v>
+      </c>
+      <c r="C29" t="s">
         <v>235</v>
       </c>
-      <c r="B29" t="s">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>234</v>
+      </c>
+      <c r="B30" t="s">
+        <v>380</v>
+      </c>
+      <c r="C30" t="s">
         <v>236</v>
       </c>
-      <c r="C29" t="s">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>234</v>
+      </c>
+      <c r="B31" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
-        <v>235</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="C31" t="s">
         <v>238</v>
       </c>
-      <c r="C30" t="s">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>234</v>
+      </c>
+      <c r="B32" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
-        <v>235</v>
-      </c>
-      <c r="B31" t="s">
+      <c r="C32" t="s">
         <v>240</v>
       </c>
-      <c r="C31" t="s">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>234</v>
+      </c>
+      <c r="B33" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" t="s">
-        <v>235</v>
-      </c>
-      <c r="B32" t="s">
+      <c r="C33" t="s">
         <v>242</v>
       </c>
-      <c r="C32" t="s">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>234</v>
+      </c>
+      <c r="B34" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
-        <v>235</v>
-      </c>
-      <c r="B33" t="s">
+      <c r="C34" t="s">
         <v>244</v>
       </c>
-      <c r="C33" t="s">
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>234</v>
+      </c>
+      <c r="B35" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
-        <v>235</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="C35" t="s">
         <v>246</v>
       </c>
-      <c r="C34" t="s">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>234</v>
+      </c>
+      <c r="B36" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
-        <v>235</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="C36" t="s">
         <v>248</v>
       </c>
-      <c r="C35" t="s">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>234</v>
+      </c>
+      <c r="B37" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
-        <v>235</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="C37" t="s">
         <v>250</v>
       </c>
-      <c r="C36" t="s">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>234</v>
+      </c>
+      <c r="B38" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
-        <v>235</v>
-      </c>
-      <c r="B37" t="s">
+      <c r="C38" t="s">
         <v>252</v>
       </c>
-      <c r="C37" t="s">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" t="s">
-        <v>235</v>
-      </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>254</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
-      <c r="A39" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>253</v>
+      </c>
+      <c r="B40" t="s">
         <v>256</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C40" t="s">
         <v>257</v>
       </c>
-      <c r="C39" t="s">
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>253</v>
+      </c>
+      <c r="B41" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" t="s">
-        <v>256</v>
-      </c>
-      <c r="B40" t="s">
+      <c r="C41" t="s">
         <v>259</v>
       </c>
-      <c r="C40" t="s">
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>253</v>
+      </c>
+      <c r="B42" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" t="s">
-        <v>256</v>
-      </c>
-      <c r="B41" t="s">
+      <c r="C42" t="s">
         <v>261</v>
       </c>
-      <c r="C41" t="s">
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>253</v>
+      </c>
+      <c r="B43" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" t="s">
-        <v>256</v>
-      </c>
-      <c r="B42" t="s">
+      <c r="C43" t="s">
         <v>263</v>
       </c>
-      <c r="C42" t="s">
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" t="s">
-        <v>256</v>
-      </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>265</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
-      <c r="A44" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>264</v>
+      </c>
+      <c r="B45" t="s">
         <v>267</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C45" t="s">
         <v>268</v>
       </c>
-      <c r="C44" t="s">
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>264</v>
+      </c>
+      <c r="B46" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" t="s">
-        <v>267</v>
-      </c>
-      <c r="B45" t="s">
+      <c r="C46" t="s">
         <v>270</v>
       </c>
-      <c r="C45" t="s">
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>264</v>
+      </c>
+      <c r="B47" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" t="s">
-        <v>267</v>
-      </c>
-      <c r="B46" t="s">
+      <c r="C47" t="s">
         <v>272</v>
       </c>
-      <c r="C46" t="s">
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>264</v>
+      </c>
+      <c r="B48" t="s">
+        <v>262</v>
+      </c>
+      <c r="C48" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" t="s">
-        <v>267</v>
-      </c>
-      <c r="B47" t="s">
+      <c r="B49" t="s">
         <v>274</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C49" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
-      <c r="A48" t="s">
-        <v>267</v>
-      </c>
-      <c r="B48" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>273</v>
+      </c>
+      <c r="B50" t="s">
         <v>276</v>
       </c>
-      <c r="C48" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" t="s">
+      <c r="C50" t="s">
         <v>277</v>
       </c>
-      <c r="B49" t="s">
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>273</v>
+      </c>
+      <c r="B51" t="s">
         <v>278</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C51" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
-      <c r="A50" t="s">
-        <v>277</v>
-      </c>
-      <c r="B50" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>273</v>
+      </c>
+      <c r="B52" t="s">
         <v>280</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C52" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
-      <c r="A51" t="s">
-        <v>277</v>
-      </c>
-      <c r="B51" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>273</v>
+      </c>
+      <c r="B53" t="s">
         <v>282</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C53" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
-      <c r="A52" t="s">
-        <v>277</v>
-      </c>
-      <c r="B52" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>273</v>
+      </c>
+      <c r="B54" t="s">
         <v>284</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C54" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
-      <c r="A53" t="s">
-        <v>277</v>
-      </c>
-      <c r="B53" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>273</v>
+      </c>
+      <c r="B55" t="s">
         <v>286</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C55" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
-      <c r="A54" t="s">
-        <v>277</v>
-      </c>
-      <c r="B54" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>273</v>
+      </c>
+      <c r="B56" t="s">
+        <v>199</v>
+      </c>
+      <c r="C56" t="s">
         <v>288</v>
       </c>
-      <c r="C54" t="s">
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" t="s">
-        <v>277</v>
-      </c>
-      <c r="B55" t="s">
+      <c r="B57" t="s">
+        <v>399</v>
+      </c>
+      <c r="C57" t="s">
         <v>290</v>
       </c>
-      <c r="C55" t="s">
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>289</v>
+      </c>
+      <c r="B58" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" t="s">
-        <v>277</v>
-      </c>
-      <c r="B56" t="s">
-        <v>200</v>
-      </c>
-      <c r="C56" t="s">
+      <c r="C58" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
-      <c r="A57" t="s">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>289</v>
+      </c>
+      <c r="B59" t="s">
         <v>293</v>
       </c>
-      <c r="B57" t="s">
-        <v>182</v>
-      </c>
-      <c r="C57" t="s">
+      <c r="C59" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
-      <c r="A58" t="s">
-        <v>293</v>
-      </c>
-      <c r="B58" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>289</v>
+      </c>
+      <c r="B60" t="s">
         <v>295</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C60" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
-      <c r="A59" t="s">
-        <v>293</v>
-      </c>
-      <c r="B59" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>289</v>
+      </c>
+      <c r="B61" t="s">
         <v>297</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C61" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
-      <c r="A60" t="s">
-        <v>293</v>
-      </c>
-      <c r="B60" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>289</v>
+      </c>
+      <c r="B62" t="s">
         <v>299</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C62" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
-      <c r="A61" t="s">
-        <v>293</v>
-      </c>
-      <c r="B61" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>289</v>
+      </c>
+      <c r="B63" t="s">
         <v>301</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C63" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
-      <c r="A62" t="s">
-        <v>293</v>
-      </c>
-      <c r="B62" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>289</v>
+      </c>
+      <c r="B64" t="s">
         <v>303</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C64" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
-      <c r="A63" t="s">
-        <v>293</v>
-      </c>
-      <c r="B63" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>289</v>
+      </c>
+      <c r="B65" t="s">
         <v>305</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C65" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
-      <c r="A64" t="s">
-        <v>293</v>
-      </c>
-      <c r="B64" t="s">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>307</v>
-      </c>
-      <c r="C64" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" t="s">
-        <v>293</v>
-      </c>
-      <c r="B65" t="s">
-        <v>309</v>
-      </c>
-      <c r="C65" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" t="s">
-        <v>311</v>
       </c>
       <c r="B66" t="s">
         <v>177</v>
@@ -3421,548 +3492,548 @@
         <v>178</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B67" t="s">
         <v>179</v>
       </c>
       <c r="C67" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>309</v>
+      </c>
+      <c r="B68" t="s">
+        <v>310</v>
+      </c>
+      <c r="C68" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>309</v>
+      </c>
+      <c r="B69" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" t="s">
+      <c r="C69" t="s">
         <v>313</v>
       </c>
-      <c r="B68" t="s">
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>309</v>
+      </c>
+      <c r="B70" t="s">
         <v>314</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C70" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
-      <c r="A69" t="s">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>309</v>
+      </c>
+      <c r="B71" t="s">
+        <v>382</v>
+      </c>
+      <c r="C71" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>317</v>
+      </c>
+      <c r="B72" t="s">
+        <v>310</v>
+      </c>
+      <c r="C72" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>317</v>
+      </c>
+      <c r="B73" t="s">
+        <v>312</v>
+      </c>
+      <c r="C73" t="s">
         <v>313</v>
       </c>
-      <c r="B69" t="s">
-        <v>316</v>
-      </c>
-      <c r="C69" t="s">
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70" t="s">
-        <v>313</v>
-      </c>
-      <c r="B70" t="s">
+      <c r="B74" t="s">
+        <v>314</v>
+      </c>
+      <c r="C74" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>317</v>
+      </c>
+      <c r="B75" t="s">
+        <v>382</v>
+      </c>
+      <c r="C75" t="s">
         <v>318</v>
       </c>
-      <c r="C70" t="s">
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" t="s">
-        <v>313</v>
-      </c>
-      <c r="B71" t="s">
+      <c r="B76" t="s">
+        <v>400</v>
+      </c>
+      <c r="C76" t="s">
         <v>320</v>
       </c>
-      <c r="C71" t="s">
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>319</v>
+      </c>
+      <c r="B77" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" t="s">
+      <c r="C77" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>319</v>
+      </c>
+      <c r="B78" t="s">
         <v>322</v>
       </c>
-      <c r="B72" t="s">
-        <v>314</v>
-      </c>
-      <c r="C72" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73" t="s">
-        <v>322</v>
-      </c>
-      <c r="B73" t="s">
-        <v>316</v>
-      </c>
-      <c r="C73" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" t="s">
-        <v>322</v>
-      </c>
-      <c r="B74" t="s">
-        <v>318</v>
-      </c>
-      <c r="C74" t="s">
+      <c r="C78" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75" t="s">
-        <v>322</v>
-      </c>
-      <c r="B75" t="s">
-        <v>320</v>
-      </c>
-      <c r="C75" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="A76" t="s">
+      <c r="B79" t="s">
         <v>324</v>
       </c>
-      <c r="B76" t="s">
-        <v>182</v>
-      </c>
-      <c r="C76" t="s">
+      <c r="C79" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>319</v>
+      </c>
+      <c r="B80" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="A77" t="s">
-        <v>324</v>
-      </c>
-      <c r="B77" t="s">
+      <c r="C80" t="s">
         <v>326</v>
       </c>
-      <c r="C77" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="A78" t="s">
-        <v>324</v>
-      </c>
-      <c r="B78" t="s">
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
         <v>327</v>
       </c>
-      <c r="C78" t="s">
+      <c r="B81" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="A79" t="s">
-        <v>324</v>
-      </c>
-      <c r="B79" t="s">
+      <c r="C81" t="s">
         <v>329</v>
       </c>
-      <c r="C79" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="A80" t="s">
-        <v>324</v>
-      </c>
-      <c r="B80" t="s">
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>327</v>
+      </c>
+      <c r="B82" t="s">
         <v>330</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C82" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
-      <c r="A81" t="s">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>327</v>
+      </c>
+      <c r="B83" t="s">
+        <v>383</v>
+      </c>
+      <c r="C83" t="s">
         <v>332</v>
       </c>
-      <c r="B81" t="s">
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
         <v>333</v>
       </c>
-      <c r="C81" t="s">
+      <c r="B84" t="s">
+        <v>384</v>
+      </c>
+      <c r="C84" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
-      <c r="A82" t="s">
-        <v>332</v>
-      </c>
-      <c r="B82" t="s">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>333</v>
+      </c>
+      <c r="B85" t="s">
+        <v>385</v>
+      </c>
+      <c r="C85" t="s">
         <v>335</v>
       </c>
-      <c r="C82" t="s">
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>333</v>
+      </c>
+      <c r="B86" t="s">
+        <v>386</v>
+      </c>
+      <c r="C86" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
-      <c r="A83" t="s">
-        <v>332</v>
-      </c>
-      <c r="B83" t="s">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
         <v>337</v>
       </c>
-      <c r="C83" t="s">
+      <c r="B87" t="s">
+        <v>387</v>
+      </c>
+      <c r="C87" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
-      <c r="A84" t="s">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>337</v>
+      </c>
+      <c r="B88" t="s">
+        <v>388</v>
+      </c>
+      <c r="C88" t="s">
         <v>339</v>
       </c>
-      <c r="B84" t="s">
-        <v>333</v>
-      </c>
-      <c r="C84" t="s">
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>337</v>
+      </c>
+      <c r="B89" t="s">
+        <v>389</v>
+      </c>
+      <c r="C89" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
-      <c r="A85" t="s">
-        <v>339</v>
-      </c>
-      <c r="B85" t="s">
-        <v>335</v>
-      </c>
-      <c r="C85" t="s">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="86" spans="1:3">
-      <c r="A86" t="s">
-        <v>339</v>
-      </c>
-      <c r="B86" t="s">
-        <v>337</v>
-      </c>
-      <c r="C86" t="s">
+      <c r="B90" t="s">
+        <v>390</v>
+      </c>
+      <c r="C90" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
-      <c r="A87" t="s">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>341</v>
+      </c>
+      <c r="B91" t="s">
+        <v>391</v>
+      </c>
+      <c r="C91" t="s">
         <v>343</v>
       </c>
-      <c r="B87" t="s">
-        <v>333</v>
-      </c>
-      <c r="C87" t="s">
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>341</v>
+      </c>
+      <c r="B92" t="s">
+        <v>392</v>
+      </c>
+      <c r="C92" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
-      <c r="A88" t="s">
-        <v>343</v>
-      </c>
-      <c r="B88" t="s">
-        <v>335</v>
-      </c>
-      <c r="C88" t="s">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="89" spans="1:3">
-      <c r="A89" t="s">
-        <v>343</v>
-      </c>
-      <c r="B89" t="s">
-        <v>337</v>
-      </c>
-      <c r="C89" t="s">
+      <c r="B93" t="s">
+        <v>393</v>
+      </c>
+      <c r="C93" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
-      <c r="A90" t="s">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>345</v>
+      </c>
+      <c r="B94" t="s">
+        <v>394</v>
+      </c>
+      <c r="C94" t="s">
         <v>347</v>
       </c>
-      <c r="B90" t="s">
-        <v>333</v>
-      </c>
-      <c r="C90" t="s">
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>345</v>
+      </c>
+      <c r="B95" t="s">
+        <v>395</v>
+      </c>
+      <c r="C95" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
-      <c r="A91" t="s">
-        <v>347</v>
-      </c>
-      <c r="B91" t="s">
-        <v>335</v>
-      </c>
-      <c r="C91" t="s">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="92" spans="1:3">
-      <c r="A92" t="s">
-        <v>347</v>
-      </c>
-      <c r="B92" t="s">
-        <v>337</v>
-      </c>
-      <c r="C92" t="s">
+      <c r="B96" t="s">
+        <v>396</v>
+      </c>
+      <c r="C96" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
-      <c r="A93" t="s">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>349</v>
+      </c>
+      <c r="B97" t="s">
+        <v>397</v>
+      </c>
+      <c r="C97" t="s">
         <v>351</v>
       </c>
-      <c r="B93" t="s">
-        <v>333</v>
-      </c>
-      <c r="C93" t="s">
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>349</v>
+      </c>
+      <c r="B98" t="s">
+        <v>398</v>
+      </c>
+      <c r="C98" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
-      <c r="A94" t="s">
-        <v>351</v>
-      </c>
-      <c r="B94" t="s">
-        <v>335</v>
-      </c>
-      <c r="C94" t="s">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="95" spans="1:3">
-      <c r="A95" t="s">
-        <v>351</v>
-      </c>
-      <c r="B95" t="s">
-        <v>337</v>
-      </c>
-      <c r="C95" t="s">
+      <c r="B99" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="96" spans="1:3">
-      <c r="A96" t="s">
+      <c r="C99" t="s">
         <v>355</v>
       </c>
-      <c r="B96" t="s">
-        <v>333</v>
-      </c>
-      <c r="C96" t="s">
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>353</v>
+      </c>
+      <c r="B100" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="97" spans="1:3">
-      <c r="A97" t="s">
+      <c r="C100" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>353</v>
+      </c>
+      <c r="B101" t="s">
+        <v>358</v>
+      </c>
+      <c r="C101" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>353</v>
+      </c>
+      <c r="B102" t="s">
+        <v>360</v>
+      </c>
+      <c r="C102" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>362</v>
+      </c>
+      <c r="B103" t="s">
+        <v>354</v>
+      </c>
+      <c r="C103" t="s">
         <v>355</v>
       </c>
-      <c r="B97" t="s">
-        <v>335</v>
-      </c>
-      <c r="C97" t="s">
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>362</v>
+      </c>
+      <c r="B104" t="s">
+        <v>356</v>
+      </c>
+      <c r="C104" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
-      <c r="A98" t="s">
-        <v>355</v>
-      </c>
-      <c r="B98" t="s">
-        <v>337</v>
-      </c>
-      <c r="C98" t="s">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>362</v>
+      </c>
+      <c r="B105" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="99" spans="1:3">
-      <c r="A99" t="s">
+      <c r="C105" t="s">
         <v>359</v>
       </c>
-      <c r="B99" t="s">
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>362</v>
+      </c>
+      <c r="B106" t="s">
         <v>360</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C106" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
-      <c r="A100" t="s">
-        <v>359</v>
-      </c>
-      <c r="B100" t="s">
-        <v>362</v>
-      </c>
-      <c r="C100" t="s">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
         <v>363</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3">
-      <c r="A101" t="s">
-        <v>359</v>
-      </c>
-      <c r="B101" t="s">
-        <v>364</v>
-      </c>
-      <c r="C101" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3">
-      <c r="A102" t="s">
-        <v>359</v>
-      </c>
-      <c r="B102" t="s">
-        <v>366</v>
-      </c>
-      <c r="C102" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3">
-      <c r="A103" t="s">
-        <v>368</v>
-      </c>
-      <c r="B103" t="s">
-        <v>360</v>
-      </c>
-      <c r="C103" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3">
-      <c r="A104" t="s">
-        <v>368</v>
-      </c>
-      <c r="B104" t="s">
-        <v>362</v>
-      </c>
-      <c r="C104" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3">
-      <c r="A105" t="s">
-        <v>368</v>
-      </c>
-      <c r="B105" t="s">
-        <v>364</v>
-      </c>
-      <c r="C105" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3">
-      <c r="A106" t="s">
-        <v>368</v>
-      </c>
-      <c r="B106" t="s">
-        <v>366</v>
-      </c>
-      <c r="C106" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3">
-      <c r="A107" t="s">
-        <v>369</v>
       </c>
       <c r="B107" t="s">
         <v>179</v>
       </c>
       <c r="C107" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
+        <v>363</v>
+      </c>
+      <c r="B108" t="s">
+        <v>364</v>
+      </c>
+      <c r="C108" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>363</v>
+      </c>
+      <c r="B109" t="s">
+        <v>366</v>
+      </c>
+      <c r="C109" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>363</v>
+      </c>
+      <c r="B110" t="s">
+        <v>368</v>
+      </c>
+      <c r="C110" t="s">
         <v>369</v>
       </c>
-      <c r="B108" t="s">
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>363</v>
+      </c>
+      <c r="B111" t="s">
+        <v>199</v>
+      </c>
+      <c r="C111" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
         <v>370</v>
       </c>
-      <c r="C108" t="s">
+      <c r="B112" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="109" spans="1:3">
-      <c r="A109" t="s">
-        <v>369</v>
-      </c>
-      <c r="B109" t="s">
+      <c r="C112" t="s">
         <v>372</v>
       </c>
-      <c r="C109" t="s">
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>370</v>
+      </c>
+      <c r="B113" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="110" spans="1:3">
-      <c r="A110" t="s">
-        <v>369</v>
-      </c>
-      <c r="B110" t="s">
+      <c r="C113" t="s">
         <v>374</v>
       </c>
-      <c r="C110" t="s">
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>370</v>
+      </c>
+      <c r="B114" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="111" spans="1:3">
-      <c r="A111" t="s">
-        <v>369</v>
-      </c>
-      <c r="B111" t="s">
-        <v>200</v>
-      </c>
-      <c r="C111" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3">
-      <c r="A112" t="s">
+      <c r="C114" t="s">
         <v>376</v>
       </c>
-      <c r="B112" t="s">
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>370</v>
+      </c>
+      <c r="B115" t="s">
         <v>377</v>
       </c>
-      <c r="C112" t="s">
+      <c r="C115" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="113" spans="1:3">
-      <c r="A113" t="s">
-        <v>376</v>
-      </c>
-      <c r="B113" t="s">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
         <v>379</v>
-      </c>
-      <c r="C113" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3">
-      <c r="A114" t="s">
-        <v>376</v>
-      </c>
-      <c r="B114" t="s">
-        <v>381</v>
-      </c>
-      <c r="C114" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3">
-      <c r="A115" t="s">
-        <v>376</v>
-      </c>
-      <c r="B115" t="s">
-        <v>383</v>
-      </c>
-      <c r="C115" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3">
-      <c r="A116" t="s">
-        <v>385</v>
       </c>
       <c r="B116" t="s">
         <v>177</v>
@@ -3971,9 +4042,9 @@
         <v>177</v>
       </c>
     </row>
-    <row r="117" spans="1:3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="B117" t="s">
         <v>179</v>
@@ -3988,12 +4059,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>